<commit_message>
1001 lines, project done, waiting for partner confirmation to submit
</commit_message>
<xml_diff>
--- a/Project/Data.xlsx
+++ b/Project/Data.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardo/MEU/Programming Paradigms/finalProject/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFACA1F5-D5C8-1C43-B38D-1F774B448A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{25623F0E-AD08-3943-9BD9-C542E5089E88}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16800" windowHeight="19520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="19520" windowWidth="16800" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="197">
   <si>
     <t>player_id</t>
   </si>
@@ -618,6 +618,12 @@
   </si>
   <si>
     <t>salary</t>
+  </si>
+  <si>
+    <t>te</t>
+  </si>
+  <si>
+    <t>ts</t>
   </si>
 </sst>
 </file>
@@ -681,23 +687,23 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="6" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -714,10 +720,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -873,7 +879,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -882,13 +888,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -898,7 +904,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -907,7 +913,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -916,7 +922,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -926,12 +932,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -962,7 +968,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -981,7 +987,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -993,21 +999,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="200" workbookViewId="0">
-      <selection activeCell="E111" sqref="E111"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0" zoomScale="200">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -3031,6 +3037,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>